<commit_message>
Build 4 - Debug and Production versions
Signed-off-by: Duncan Munro <duncan@duncanamps.com>
</commit_message>
<xml_diff>
--- a/weed_todo_list.xlsx
+++ b/weed_todo_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>weed todo list</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Add quarterly option</t>
+  </si>
+  <si>
+    <t>Create debug and production versions</t>
   </si>
 </sst>
 </file>
@@ -112,8 +115,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B55B566-BA0C-40CA-A4A0-4CADED9E0CC8}" name="Table1" displayName="Table1" ref="A3:E5" totalsRowShown="0">
-  <autoFilter ref="A3:E5" xr:uid="{1F33B9B3-4997-4311-8558-95F857BE3336}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B55B566-BA0C-40CA-A4A0-4CADED9E0CC8}" name="Table1" displayName="Table1" ref="A3:E6" totalsRowShown="0">
+  <autoFilter ref="A3:E6" xr:uid="{1F33B9B3-4997-4311-8558-95F857BE3336}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{60F0FD93-206E-4E0A-94A5-12DCD1A8890F}" name="Registered" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A8B8380A-4125-41C6-8A5B-0FEAEE9AD327}" name="Item"/>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,6 +462,23 @@
         <v>42990</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42990</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>42990</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Build 6 - Improved date handling and general code cleanup
Signed-off-by: Duncan Munro <duncan@duncanamps.com>
</commit_message>
<xml_diff>
--- a/weed_todo_list.xlsx
+++ b/weed_todo_list.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>weed todo list</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Create debug and production versions</t>
+  </si>
+  <si>
+    <t>Improve code around calculating retentions</t>
+  </si>
+  <si>
+    <t>General code and function cleanup</t>
   </si>
 </sst>
 </file>
@@ -115,8 +121,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B55B566-BA0C-40CA-A4A0-4CADED9E0CC8}" name="Table1" displayName="Table1" ref="A3:E6" totalsRowShown="0">
-  <autoFilter ref="A3:E6" xr:uid="{1F33B9B3-4997-4311-8558-95F857BE3336}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B55B566-BA0C-40CA-A4A0-4CADED9E0CC8}" name="Table1" displayName="Table1" ref="A3:E8" totalsRowShown="0">
+  <autoFilter ref="A3:E8" xr:uid="{1F33B9B3-4997-4311-8558-95F857BE3336}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{60F0FD93-206E-4E0A-94A5-12DCD1A8890F}" name="Registered" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A8B8380A-4125-41C6-8A5B-0FEAEE9AD327}" name="Item"/>
@@ -391,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,6 +485,40 @@
         <v>42990</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42991</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>42991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42991</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>42991</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>